<commit_message>
new render task at 20210316
</commit_message>
<xml_diff>
--- a/cov_vac_20210316.xlsx
+++ b/cov_vac_20210316.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A2638B-C7D4-4019-A96E-D39F38816BDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5388BB2-4E2A-4AEA-944C-7DE5A6DFD8D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="108" windowWidth="28512" windowHeight="12600" tabRatio="597" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="9" r:id="rId1"/>
-    <sheet name="Gesamt_bis_einschl_14.03.21" sheetId="12" r:id="rId2"/>
-    <sheet name="Indik_bis_einschl_14.03." sheetId="11" r:id="rId3"/>
+    <sheet name="Gesamt_bis_einschl_15.03.21" sheetId="12" r:id="rId2"/>
+    <sheet name="Indik_bis_einschl_15.03." sheetId="11" r:id="rId3"/>
     <sheet name="Impfungen_proTag" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Bundesländer001" localSheetId="1">Gesamt_bis_einschl_14.03.21!#REF!</definedName>
-    <definedName name="Bundesländer001" localSheetId="2">Indik_bis_einschl_14.03.!$G$2:$J$18</definedName>
-    <definedName name="Bundesländer001_1" localSheetId="1">Gesamt_bis_einschl_14.03.21!$D$3:$H$19</definedName>
-    <definedName name="Bundesländer001_1" localSheetId="2">Indik_bis_einschl_14.03.!$C$2:$F$18</definedName>
+    <definedName name="Bundesländer001" localSheetId="1">Gesamt_bis_einschl_15.03.21!#REF!</definedName>
+    <definedName name="Bundesländer001" localSheetId="2">Indik_bis_einschl_15.03.!$G$2:$J$18</definedName>
+    <definedName name="Bundesländer001_1" localSheetId="1">Gesamt_bis_einschl_15.03.21!$D$3:$H$19</definedName>
+    <definedName name="Bundesländer001_1" localSheetId="2">Indik_bis_einschl_15.03.!$C$2:$F$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
   <si>
     <t>Bayern</t>
   </si>
@@ -217,34 +217,28 @@
     <t>Bund *</t>
   </si>
   <si>
-    <t>* Impfungen, die in den bundeseigenen Impfzentren aus dem Impfkontingent des Bundes durchgeführt wurden. Diese gehen in die Berechnung der Impfquote für Gesamtdeutschland mit ein und umfassen nur Angehörige des Bundes, die nach §§ 2, 3 und 4 Coronavirus-Impfverordnung geimpft wurden. Die Impfungen sind erfasst, die Impfdaten befinden sich in Abstimmung.</t>
-  </si>
-  <si>
-    <t>** Impfungen, die in den bundeseigenen Impfzentren aus dem Impfkontingent des Bundes durchgeführt wurden. Diese gehen in die Berechnung der Impfquote für Gesamtdeutschland mit ein und umfassen nur Angehörige des Bundes, die nach §§ 2, 3 und 4 Coronavirus-Impfverordnung geimpft wurden. Die Impfungen sind erfasst, die Impfdaten befinden sich in Abstimmung.</t>
-  </si>
-  <si>
     <t>Bund **</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t xml:space="preserve">Die kumulative Zahl der Impfungen umfasst alle Impfungen, die bis einschließlich 12.03.21 durchgeführt und bis zum 13.03.21, 8:00 Uhr, dem RKI gemeldet wurden. Nachmeldungen und Datenkorrekturen aus zurückliegenden Tagen sind in der kumulativen Zahl der Impfungen enthalten. </t>
-  </si>
-  <si>
-    <t>Datenstand: 15.03.2021, 8:00 Uhr</t>
-  </si>
-  <si>
-    <t>Durchgeführte Impfungen bundesweit und nach Bundesland bis einschließlich 14.03.21 (Gesamt_bis_einschl_14.03.21)</t>
-  </si>
-  <si>
-    <t>Anzahl Impfungen nach Indikation bis einschließlich 14.03.21 (Indik_bis_einschl_14.03.21)</t>
-  </si>
-  <si>
-    <t>Nordrhein-Westfalen **</t>
-  </si>
-  <si>
-    <t>** Die Daten enthalten nachträgliche Korrekturen aus Nordrhein-Westfalen.</t>
+    <t>Datenstand: 16.03.2021, 8:00 Uhr</t>
+  </si>
+  <si>
+    <t>Durchgeführte Impfungen bundesweit und nach Bundesland bis einschließlich 15.03.21 (Gesamt_bis_einschl_15.03.21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die kumulative Zahl der Impfungen umfasst alle Impfungen, die bis einschließlich 15.03.21 durchgeführt und bis zum 16.03.21, 8:00 Uhr, dem RKI gemeldet wurden. Nachmeldungen und Datenkorrekturen aus zurückliegenden Tagen sind in der kumulativen Zahl der Impfungen enthalten. </t>
+  </si>
+  <si>
+    <t>Anzahl Impfungen nach Indikation bis einschließlich 15.03.21 (Indik_bis_einschl_15.03.21)</t>
+  </si>
+  <si>
+    <t>** Impfungen, die in den bundeseigenen Impfzentren aus dem Impfkontingent des Bundes durchgeführt wurden. Diese gehen in die Berechnung der Impfquote für Gesamtdeutschland mit ein und umfassen nur Angehörige des Bundes, die nach §§ 2, 3 und 4 Coronavirus-Impfverordnung geimpft wurden. Die Zahlen werden wöchentlich jeweils montags aktualisiert.</t>
+  </si>
+  <si>
+    <t>* Impfungen, die in den bundeseigenen Impfzentren aus dem Impfkontingent des Bundes durchgeführt wurden. Diese gehen in die Berechnung der Impfquote für Gesamtdeutschland mit ein und umfassen nur Angehörige des Bundes, die nach §§ 2, 3 und 4 Coronavirus-Impfverordnung geimpft wurden. Die Zahlen werden wöchentlich jeweils montags aktualisiert.</t>
   </si>
 </sst>
 </file>
@@ -698,12 +692,12 @@
     <xf numFmtId="3" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -813,7 +807,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001" fillFormulas="1" connectionId="1" xr16:uid="{8C6643A4-82D3-4F11-ADE7-BA4132573BCB}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001_1" fillFormulas="1" connectionId="2" xr16:uid="{85D177FD-4909-4AAF-B663-F45CEC25E8F5}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="13">
     <queryTableFields count="4">
       <queryTableField id="5" name="Fälle in den letzten 7 Tagen"/>
@@ -834,7 +828,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001_1" fillFormulas="1" connectionId="2" xr16:uid="{85D177FD-4909-4AAF-B663-F45CEC25E8F5}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001" fillFormulas="1" connectionId="1" xr16:uid="{8C6643A4-82D3-4F11-ADE7-BA4132573BCB}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="13">
     <queryTableFields count="4">
       <queryTableField id="5" name="Fälle in den letzten 7 Tagen"/>
@@ -1177,7 +1171,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5241AA5B-8CBB-47B1-9317-352256D0A517}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1197,7 +1193,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -1209,7 +1205,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1235,7 +1231,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1300,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A1EB7E-F725-49E9-9B87-E64B6D1D2BBC}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1419,43 +1415,43 @@
         <v>1</v>
       </c>
       <c r="C4" s="26">
-        <v>1243998</v>
+        <v>1276282</v>
       </c>
       <c r="D4" s="10">
-        <v>858236</v>
+        <v>883965</v>
       </c>
       <c r="E4" s="10">
-        <v>576255</v>
+        <v>588993</v>
       </c>
       <c r="F4" s="10">
-        <v>36911</v>
+        <v>38096</v>
       </c>
       <c r="G4" s="10">
-        <v>245070</v>
+        <v>256876</v>
       </c>
       <c r="H4" s="10">
-        <v>21548</v>
+        <v>24853</v>
       </c>
       <c r="I4" s="25">
-        <v>7.7315814195424046</v>
+        <v>7.9633659850271989</v>
       </c>
       <c r="J4" s="22">
-        <v>385762</v>
+        <v>392317</v>
       </c>
       <c r="K4" s="10">
-        <v>371084</v>
+        <v>377496</v>
       </c>
       <c r="L4" s="10">
-        <v>14674</v>
+        <v>14817</v>
       </c>
       <c r="M4" s="10">
         <v>4</v>
       </c>
       <c r="N4" s="11">
-        <v>6079</v>
+        <v>6544</v>
       </c>
       <c r="O4" s="42">
-        <v>3.4752099790331767</v>
+        <v>3.5342619370087225</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1466,43 +1462,43 @@
         <v>0</v>
       </c>
       <c r="C5" s="27">
-        <v>1621834</v>
+        <v>1663320</v>
       </c>
       <c r="D5" s="15">
-        <v>1116691</v>
+        <v>1147115</v>
       </c>
       <c r="E5" s="15">
-        <v>796237</v>
+        <v>811751</v>
       </c>
       <c r="F5" s="15">
-        <v>46883</v>
+        <v>49691</v>
       </c>
       <c r="G5" s="15">
-        <v>273571</v>
+        <v>285673</v>
       </c>
       <c r="H5" s="16">
-        <v>24869</v>
+        <v>30424</v>
       </c>
       <c r="I5" s="17">
-        <v>8.5082923947352249</v>
+        <v>8.7400989444588486</v>
       </c>
       <c r="J5" s="23">
-        <v>505143</v>
+        <v>516205</v>
       </c>
       <c r="K5" s="15">
-        <v>493264</v>
+        <v>504199</v>
       </c>
       <c r="L5" s="15">
-        <v>11853</v>
+        <v>11976</v>
       </c>
       <c r="M5" s="15">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="N5" s="16">
-        <v>6683</v>
+        <v>11062</v>
       </c>
       <c r="O5" s="17">
-        <v>3.8487856937628537</v>
+        <v>3.9330692874074353</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1513,43 +1509,43 @@
         <v>3</v>
       </c>
       <c r="C6" s="26">
-        <v>437312</v>
+        <v>447470</v>
       </c>
       <c r="D6" s="10">
-        <v>295039</v>
+        <v>303637</v>
       </c>
       <c r="E6" s="10">
-        <v>219692</v>
+        <v>224920</v>
       </c>
       <c r="F6" s="10">
-        <v>17951</v>
+        <v>18948</v>
       </c>
       <c r="G6" s="10">
-        <v>57396</v>
+        <v>59769</v>
       </c>
       <c r="H6" s="11">
-        <v>9153</v>
+        <v>8598</v>
       </c>
       <c r="I6" s="12">
-        <v>8.0403249387994133</v>
+        <v>8.2746353649593356</v>
       </c>
       <c r="J6" s="22">
-        <v>142273</v>
+        <v>143833</v>
       </c>
       <c r="K6" s="10">
-        <v>138149</v>
+        <v>139683</v>
       </c>
       <c r="L6" s="10">
-        <v>4124</v>
+        <v>4150</v>
       </c>
       <c r="M6" s="10">
         <v>0</v>
       </c>
       <c r="N6" s="11">
-        <v>1623</v>
+        <v>1560</v>
       </c>
       <c r="O6" s="12">
-        <v>3.877186236456228</v>
+        <v>3.9196989446220201</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1560,31 +1556,31 @@
         <v>2</v>
       </c>
       <c r="C7" s="27">
-        <v>261971</v>
+        <v>268143</v>
       </c>
       <c r="D7" s="15">
-        <v>181451</v>
+        <v>187196</v>
       </c>
       <c r="E7" s="15">
-        <v>112291</v>
+        <v>115672</v>
       </c>
       <c r="F7" s="15">
-        <v>8780</v>
+        <v>9527</v>
       </c>
       <c r="G7" s="15">
-        <v>60380</v>
+        <v>61997</v>
       </c>
       <c r="H7" s="16">
-        <v>61</v>
+        <v>5845</v>
       </c>
       <c r="I7" s="17">
-        <v>7.1950316686711133</v>
+        <v>7.4228367341516872</v>
       </c>
       <c r="J7" s="23">
-        <v>80520</v>
+        <v>80947</v>
       </c>
       <c r="K7" s="15">
-        <v>76448</v>
+        <v>76875</v>
       </c>
       <c r="L7" s="15">
         <v>4071</v>
@@ -1593,10 +1589,10 @@
         <v>1</v>
       </c>
       <c r="N7" s="16">
-        <v>52</v>
+        <v>427</v>
       </c>
       <c r="O7" s="17">
-        <v>3.1928396644901271</v>
+        <v>3.2097713899836351</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1607,31 +1603,31 @@
         <v>4</v>
       </c>
       <c r="C8" s="26">
-        <v>85720</v>
+        <v>87671</v>
       </c>
       <c r="D8" s="10">
-        <v>60139</v>
+        <v>61555</v>
       </c>
       <c r="E8" s="10">
-        <v>38137</v>
+        <v>38555</v>
       </c>
       <c r="F8" s="10">
         <v>3037</v>
       </c>
       <c r="G8" s="10">
-        <v>18965</v>
+        <v>19963</v>
       </c>
       <c r="H8" s="11">
-        <v>903</v>
+        <v>1416</v>
       </c>
       <c r="I8" s="12">
-        <v>8.8283651545356587</v>
+        <v>9.0362330116470595</v>
       </c>
       <c r="J8" s="22">
-        <v>25581</v>
+        <v>26116</v>
       </c>
       <c r="K8" s="10">
-        <v>24271</v>
+        <v>24806</v>
       </c>
       <c r="L8" s="10">
         <v>1310</v>
@@ -1640,10 +1636,10 @@
         <v>0</v>
       </c>
       <c r="N8" s="11">
-        <v>269</v>
+        <v>535</v>
       </c>
       <c r="O8" s="12">
-        <v>3.7552737660781972</v>
+        <v>3.8338114098314455</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -1654,43 +1650,43 @@
         <v>5</v>
       </c>
       <c r="C9" s="27">
-        <v>222122</v>
+        <v>227150</v>
       </c>
       <c r="D9" s="15">
-        <v>151821</v>
+        <v>155380</v>
       </c>
       <c r="E9" s="15">
-        <v>99697</v>
+        <v>101356</v>
       </c>
       <c r="F9" s="15">
-        <v>6773</v>
+        <v>6985</v>
       </c>
       <c r="G9" s="15">
-        <v>45351</v>
+        <v>47039</v>
       </c>
       <c r="H9" s="16">
-        <v>3564</v>
+        <v>3403</v>
       </c>
       <c r="I9" s="17">
-        <v>8.2187442651331466</v>
+        <v>8.4114087241974964</v>
       </c>
       <c r="J9" s="23">
-        <v>70301</v>
+        <v>71770</v>
       </c>
       <c r="K9" s="15">
-        <v>68710</v>
+        <v>70176</v>
       </c>
       <c r="L9" s="15">
-        <v>1591</v>
+        <v>1593</v>
       </c>
       <c r="M9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="16">
-        <v>1369</v>
+        <v>1464</v>
       </c>
       <c r="O9" s="17">
-        <v>3.8057050117119848</v>
+        <v>3.8852284987492243</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -1701,43 +1697,43 @@
         <v>15</v>
       </c>
       <c r="C10" s="26">
-        <v>707427</v>
+        <v>728335</v>
       </c>
       <c r="D10" s="10">
-        <v>498552</v>
+        <v>514218</v>
       </c>
       <c r="E10" s="10">
-        <v>366593</v>
+        <v>375533</v>
       </c>
       <c r="F10" s="10">
-        <v>17256</v>
+        <v>17933</v>
       </c>
       <c r="G10" s="10">
-        <v>114703</v>
+        <v>120752</v>
       </c>
       <c r="H10" s="11">
-        <v>14849</v>
+        <v>15041</v>
       </c>
       <c r="I10" s="12">
-        <v>7.9285250823780862</v>
+        <v>8.177663134056818</v>
       </c>
       <c r="J10" s="22">
-        <v>208875</v>
+        <v>214117</v>
       </c>
       <c r="K10" s="10">
-        <v>205437</v>
+        <v>210329</v>
       </c>
       <c r="L10" s="10">
-        <v>3395</v>
+        <v>3740</v>
       </c>
       <c r="M10" s="10">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="N10" s="11">
-        <v>3530</v>
+        <v>5066</v>
       </c>
       <c r="O10" s="12">
-        <v>3.3217611735219656</v>
+        <v>3.4051252528593783</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -1748,43 +1744,43 @@
         <v>6</v>
       </c>
       <c r="C11" s="28">
-        <v>174037</v>
+        <v>178174</v>
       </c>
       <c r="D11" s="15">
-        <v>116554</v>
+        <v>119881</v>
       </c>
       <c r="E11" s="15">
-        <v>90996</v>
+        <v>92504</v>
       </c>
       <c r="F11" s="15">
-        <v>6320</v>
+        <v>6328</v>
       </c>
       <c r="G11" s="15">
-        <v>19238</v>
+        <v>21049</v>
       </c>
       <c r="H11" s="16">
-        <v>0</v>
+        <v>2843</v>
       </c>
       <c r="I11" s="17">
-        <v>7.2477610752311055</v>
+        <v>7.4546463052300238</v>
       </c>
       <c r="J11" s="23">
-        <v>57483</v>
+        <v>58293</v>
       </c>
       <c r="K11" s="15">
-        <v>56114</v>
+        <v>56764</v>
       </c>
       <c r="L11" s="15">
-        <v>1359</v>
+        <v>1516</v>
       </c>
       <c r="M11" s="15">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="N11" s="16">
-        <v>0</v>
+        <v>771</v>
       </c>
       <c r="O11" s="17">
-        <v>3.5745066654727395</v>
+        <v>3.624875477104577</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -1795,43 +1791,43 @@
         <v>7</v>
       </c>
       <c r="C12" s="26">
-        <v>830323</v>
+        <v>868874</v>
       </c>
       <c r="D12" s="10">
-        <v>577494</v>
+        <v>606701</v>
       </c>
       <c r="E12" s="10">
-        <v>422980</v>
+        <v>427327</v>
       </c>
       <c r="F12" s="10">
-        <v>19965</v>
+        <v>21851</v>
       </c>
       <c r="G12" s="10">
-        <v>134549</v>
+        <v>157523</v>
       </c>
       <c r="H12" s="11">
-        <v>3614</v>
+        <v>12909</v>
       </c>
       <c r="I12" s="12">
-        <v>7.2244473334194019</v>
+        <v>7.5898267715905003</v>
       </c>
       <c r="J12" s="22">
-        <v>252829</v>
+        <v>262173</v>
       </c>
       <c r="K12" s="10">
-        <v>248243</v>
+        <v>257429</v>
       </c>
       <c r="L12" s="10">
-        <v>4586</v>
+        <v>4744</v>
       </c>
       <c r="M12" s="10">
         <v>0</v>
       </c>
       <c r="N12" s="11">
-        <v>439</v>
+        <v>9000</v>
       </c>
       <c r="O12" s="12">
-        <v>3.1628896488294145</v>
+        <v>3.279783046654277</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -1839,46 +1835,46 @@
         <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C13" s="27">
-        <v>1937317</v>
+        <v>1989474</v>
       </c>
       <c r="D13" s="15">
-        <v>1343693</v>
+        <v>1384577</v>
       </c>
       <c r="E13" s="15">
-        <v>968456</v>
+        <v>986740</v>
       </c>
       <c r="F13" s="15">
-        <v>29142</v>
+        <v>29677</v>
       </c>
       <c r="G13" s="15">
-        <v>346095</v>
+        <v>368160</v>
       </c>
       <c r="H13" s="16">
-        <v>28631</v>
+        <v>24382</v>
       </c>
       <c r="I13" s="17">
-        <v>7.4869139907509918</v>
+        <v>7.7147152754178494</v>
       </c>
       <c r="J13" s="23">
-        <v>593624</v>
+        <v>604897</v>
       </c>
       <c r="K13" s="15">
-        <v>579865</v>
+        <v>591120</v>
       </c>
       <c r="L13" s="15">
         <v>13638</v>
       </c>
       <c r="M13" s="15">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="N13" s="16">
-        <v>9468</v>
+        <v>9704</v>
       </c>
       <c r="O13" s="17">
-        <v>3.3076095736493132</v>
+        <v>3.3704215265416302</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -1889,43 +1885,43 @@
         <v>12</v>
       </c>
       <c r="C14" s="26">
-        <v>479515</v>
+        <v>494287</v>
       </c>
       <c r="D14" s="10">
-        <v>335544</v>
+        <v>349682</v>
       </c>
       <c r="E14" s="10">
-        <v>214110</v>
+        <v>221462</v>
       </c>
       <c r="F14" s="10">
-        <v>4573</v>
+        <v>5152</v>
       </c>
       <c r="G14" s="10">
-        <v>116861</v>
+        <v>123068</v>
       </c>
       <c r="H14" s="11">
-        <v>293</v>
+        <v>13335</v>
       </c>
       <c r="I14" s="12">
-        <v>8.1961883317704398</v>
+        <v>8.5415311501029691</v>
       </c>
       <c r="J14" s="22">
-        <v>143971</v>
+        <v>144605</v>
       </c>
       <c r="K14" s="10">
-        <v>140086</v>
+        <v>140175</v>
       </c>
       <c r="L14" s="10">
-        <v>3885</v>
+        <v>4430</v>
       </c>
       <c r="M14" s="10">
         <v>0</v>
       </c>
       <c r="N14" s="11">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="O14" s="12">
-        <v>3.5167174210038685</v>
+        <v>3.5322038651135603</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -1936,43 +1932,43 @@
         <v>13</v>
       </c>
       <c r="C15" s="27">
-        <v>118742</v>
+        <v>122722</v>
       </c>
       <c r="D15" s="15">
-        <v>85970</v>
+        <v>89244</v>
       </c>
       <c r="E15" s="15">
-        <v>58333</v>
+        <v>60115</v>
       </c>
       <c r="F15" s="15">
-        <v>3390</v>
+        <v>3654</v>
       </c>
       <c r="G15" s="15">
-        <v>24247</v>
+        <v>25475</v>
       </c>
       <c r="H15" s="16">
-        <v>0</v>
+        <v>3223</v>
       </c>
       <c r="I15" s="17">
-        <v>8.7112303637599844</v>
+        <v>9.0429806046690242</v>
       </c>
       <c r="J15" s="23">
-        <v>32772</v>
+        <v>33478</v>
       </c>
       <c r="K15" s="15">
-        <v>31453</v>
+        <v>32150</v>
       </c>
       <c r="L15" s="15">
-        <v>1319</v>
+        <v>1328</v>
       </c>
       <c r="M15" s="15">
         <v>0</v>
       </c>
       <c r="N15" s="16">
-        <v>0</v>
+        <v>706</v>
       </c>
       <c r="O15" s="17">
-        <v>3.3207449282440646</v>
+        <v>3.3922830070717316</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -1983,46 +1979,46 @@
         <v>9</v>
       </c>
       <c r="C16" s="26">
-        <v>454151</v>
+        <v>463529</v>
       </c>
       <c r="D16" s="10">
-        <v>313493</v>
+        <v>317780</v>
       </c>
       <c r="E16" s="10">
-        <v>261632</v>
+        <v>263186</v>
       </c>
       <c r="F16" s="10">
-        <v>14053</v>
+        <v>14236</v>
       </c>
       <c r="G16" s="10">
-        <v>37808</v>
+        <v>40358</v>
       </c>
       <c r="H16" s="11">
-        <v>5212</v>
+        <v>4287</v>
       </c>
       <c r="I16" s="12">
-        <v>7.6988023735925433</v>
+        <v>7.8040830840887612</v>
       </c>
       <c r="J16" s="22">
-        <v>140658</v>
+        <v>145749</v>
       </c>
       <c r="K16" s="10">
-        <v>138467</v>
+        <v>143209</v>
       </c>
       <c r="L16" s="10">
-        <v>2191</v>
+        <v>2540</v>
       </c>
       <c r="M16" s="10">
         <v>0</v>
       </c>
       <c r="N16" s="11">
-        <v>5512</v>
+        <v>5091</v>
       </c>
       <c r="O16" s="12">
-        <v>3.4542976853224152</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+        <v>3.5793231336863651</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -2030,46 +2026,46 @@
         <v>10</v>
       </c>
       <c r="C17" s="27">
-        <v>223984</v>
+        <v>231603</v>
       </c>
       <c r="D17" s="15">
-        <v>155562</v>
+        <v>161437</v>
       </c>
       <c r="E17" s="15">
-        <v>104850</v>
+        <v>107623</v>
       </c>
       <c r="F17" s="15">
-        <v>8020</v>
+        <v>8447</v>
       </c>
       <c r="G17" s="15">
-        <v>42692</v>
+        <v>45367</v>
       </c>
       <c r="H17" s="16">
-        <v>1647</v>
+        <v>5875</v>
       </c>
       <c r="I17" s="17">
-        <v>7.0878109989967113</v>
+        <v>7.3554913426481532</v>
       </c>
       <c r="J17" s="23">
-        <v>68422</v>
+        <v>70166</v>
       </c>
       <c r="K17" s="15">
-        <v>66728</v>
+        <v>68469</v>
       </c>
       <c r="L17" s="15">
-        <v>1694</v>
+        <v>1697</v>
       </c>
       <c r="M17" s="15">
         <v>0</v>
       </c>
       <c r="N17" s="16">
-        <v>6</v>
+        <v>1744</v>
       </c>
       <c r="O17" s="17">
-        <v>3.1174850167351473</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+        <v>3.1969462115144012</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>41</v>
       </c>
@@ -2077,46 +2073,46 @@
         <v>11</v>
       </c>
       <c r="C18" s="26">
-        <v>337032</v>
+        <v>345899</v>
       </c>
       <c r="D18" s="10">
-        <v>237985</v>
+        <v>246457</v>
       </c>
       <c r="E18" s="10">
-        <v>167744</v>
+        <v>171939</v>
       </c>
       <c r="F18" s="10">
-        <v>8337</v>
+        <v>9271</v>
       </c>
       <c r="G18" s="10">
-        <v>61904</v>
+        <v>65247</v>
       </c>
       <c r="H18" s="11">
-        <v>5975</v>
+        <v>8347</v>
       </c>
       <c r="I18" s="12">
-        <v>8.195716400696611</v>
+        <v>8.4874747440657394</v>
       </c>
       <c r="J18" s="22">
-        <v>99047</v>
+        <v>99442</v>
       </c>
       <c r="K18" s="10">
-        <v>96948</v>
+        <v>97191</v>
       </c>
       <c r="L18" s="10">
-        <v>2087</v>
+        <v>2237</v>
       </c>
       <c r="M18" s="10">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N18" s="11">
-        <v>67</v>
+        <v>228</v>
       </c>
       <c r="O18" s="12">
-        <v>3.4109759957131636</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+        <v>3.4245789874070738</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>16</v>
       </c>
@@ -2124,31 +2120,31 @@
         <v>14</v>
       </c>
       <c r="C19" s="27">
-        <v>263625</v>
+        <v>270954</v>
       </c>
       <c r="D19" s="15">
-        <v>178935</v>
+        <v>183370</v>
       </c>
       <c r="E19" s="15">
-        <v>121941</v>
+        <v>124809</v>
       </c>
       <c r="F19" s="15">
         <v>8314</v>
       </c>
       <c r="G19" s="15">
-        <v>48680</v>
+        <v>50247</v>
       </c>
       <c r="H19" s="16">
-        <v>7829</v>
+        <v>4299</v>
       </c>
       <c r="I19" s="17">
-        <v>8.3874025137598682</v>
+        <v>8.5952887861410403</v>
       </c>
       <c r="J19" s="23">
-        <v>84690</v>
+        <v>87584</v>
       </c>
       <c r="K19" s="15">
-        <v>82012</v>
+        <v>84906</v>
       </c>
       <c r="L19" s="15">
         <v>2678</v>
@@ -2157,108 +2153,119 @@
         <v>0</v>
       </c>
       <c r="N19" s="16">
-        <v>0</v>
+        <v>2783</v>
       </c>
       <c r="O19" s="17">
-        <v>3.9697606331367439</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
+        <v>4.1054140428934769</v>
+      </c>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="55"/>
+    </row>
+    <row r="20" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>62</v>
+      <c r="C20" s="54">
+        <v>6084</v>
+      </c>
+      <c r="D20" s="10">
+        <v>6064</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="F20" s="10">
+        <v>30</v>
+      </c>
+      <c r="G20" s="10">
+        <v>6034</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="J20" s="22" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="J20" s="22">
+        <v>20</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L20" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="M20" s="10"/>
+        <v>60</v>
+      </c>
+      <c r="L20" s="10">
+        <v>20</v>
+      </c>
+      <c r="M20" s="10">
+        <v>0</v>
+      </c>
       <c r="N20" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="55"/>
+      <c r="R20" s="55"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="44"/>
       <c r="B21" s="45" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="46">
-        <v>9399110</v>
+        <v>9663887</v>
       </c>
       <c r="D21" s="44">
-        <v>6507159</v>
+        <v>6712195</v>
       </c>
       <c r="E21" s="44">
-        <v>4619944</v>
+        <v>4712485</v>
       </c>
       <c r="F21" s="44">
-        <v>239705</v>
+        <v>251147</v>
       </c>
       <c r="G21" s="44">
-        <v>1647510</v>
+        <v>1748563</v>
       </c>
       <c r="H21" s="44">
-        <v>128148</v>
+        <v>169080</v>
       </c>
       <c r="I21" s="47">
-        <v>7.8242351077223677</v>
+        <v>8.0707712488473895</v>
       </c>
       <c r="J21" s="48">
-        <v>2891951</v>
+        <v>2951692</v>
       </c>
       <c r="K21" s="44">
-        <v>2817279</v>
+        <v>2874977</v>
       </c>
       <c r="L21" s="44">
-        <v>74455</v>
+        <v>76465</v>
       </c>
       <c r="M21" s="44">
-        <v>217</v>
+        <v>250</v>
       </c>
       <c r="N21" s="44">
-        <v>35097</v>
+        <v>56773</v>
       </c>
       <c r="O21" s="47">
-        <v>3.4772939379555363</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" s="32" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3.5491267653953518</v>
+      </c>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="55"/>
+    </row>
+    <row r="23" spans="1:18" s="32" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="56" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B24" s="56"/>
       <c r="C24" s="56"/>
@@ -2275,12 +2282,7 @@
       <c r="N24" s="56"/>
       <c r="O24" s="56"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C27" s="24"/>
     </row>
   </sheetData>
@@ -2311,7 +2313,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2384,28 +2386,28 @@
         <v>1</v>
       </c>
       <c r="C3" s="13">
-        <v>400288</v>
+        <v>409111</v>
       </c>
       <c r="D3" s="11">
-        <v>375036</v>
+        <v>387027</v>
       </c>
       <c r="E3" s="11">
-        <v>45309</v>
+        <v>48743</v>
       </c>
       <c r="F3" s="14">
-        <v>90107</v>
+        <v>91018</v>
       </c>
       <c r="G3" s="13">
-        <v>228660</v>
+        <v>233539</v>
       </c>
       <c r="H3" s="11">
-        <v>131041</v>
+        <v>132427</v>
       </c>
       <c r="I3" s="11">
-        <v>8639</v>
+        <v>8694</v>
       </c>
       <c r="J3" s="14">
-        <v>70464</v>
+        <v>71244</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2416,28 +2418,28 @@
         <v>0</v>
       </c>
       <c r="C4" s="19">
-        <v>494119</v>
+        <v>512968</v>
       </c>
       <c r="D4" s="16">
-        <v>497048</v>
+        <v>505438</v>
       </c>
       <c r="E4" s="16">
-        <v>75363</v>
+        <v>79127</v>
       </c>
       <c r="F4" s="18">
-        <v>130930</v>
+        <v>131677</v>
       </c>
       <c r="G4" s="19">
-        <v>213169</v>
+        <v>221418</v>
       </c>
       <c r="H4" s="16">
-        <v>227553</v>
+        <v>229699</v>
       </c>
       <c r="I4" s="16">
-        <v>13193</v>
+        <v>13478</v>
       </c>
       <c r="J4" s="18">
-        <v>103776</v>
+        <v>104568</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2448,28 +2450,28 @@
         <v>3</v>
       </c>
       <c r="C5" s="13">
-        <v>200279</v>
+        <v>206583</v>
       </c>
       <c r="D5" s="11">
-        <v>100193</v>
+        <v>102573</v>
       </c>
       <c r="E5" s="11">
         <v>150</v>
       </c>
       <c r="F5" s="14">
-        <v>44375</v>
+        <v>45126</v>
       </c>
       <c r="G5" s="13">
-        <v>107424</v>
+        <v>108724</v>
       </c>
       <c r="H5" s="11">
-        <v>33146</v>
+        <v>33444</v>
       </c>
       <c r="I5" s="11">
         <v>30</v>
       </c>
       <c r="J5" s="14">
-        <v>38865</v>
+        <v>39061</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2480,28 +2482,28 @@
         <v>2</v>
       </c>
       <c r="C6" s="19">
-        <v>75063</v>
+        <v>78339</v>
       </c>
       <c r="D6" s="16">
-        <v>91273</v>
+        <v>92542</v>
       </c>
       <c r="E6" s="16">
-        <v>13788</v>
+        <v>15116</v>
       </c>
       <c r="F6" s="18">
-        <v>24687</v>
+        <v>25004</v>
       </c>
       <c r="G6" s="19">
-        <v>37249</v>
+        <v>37637</v>
       </c>
       <c r="H6" s="16">
-        <v>41613</v>
+        <v>41649</v>
       </c>
       <c r="I6" s="16">
-        <v>1250</v>
+        <v>1254</v>
       </c>
       <c r="J6" s="18">
-        <v>17647</v>
+        <v>17706</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2512,28 +2514,28 @@
         <v>4</v>
       </c>
       <c r="C7" s="13">
-        <v>24673</v>
+        <v>24893</v>
       </c>
       <c r="D7" s="11">
-        <v>30308</v>
+        <v>31416</v>
       </c>
       <c r="E7" s="11">
-        <v>1371</v>
+        <v>1400</v>
       </c>
       <c r="F7" s="14">
-        <v>8602</v>
+        <v>8650</v>
       </c>
       <c r="G7" s="13">
-        <v>12902</v>
+        <v>13307</v>
       </c>
       <c r="H7" s="11">
-        <v>9573</v>
+        <v>9683</v>
       </c>
       <c r="I7" s="11">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="J7" s="14">
-        <v>7158</v>
+        <v>7170</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2544,28 +2546,28 @@
         <v>5</v>
       </c>
       <c r="C8" s="19">
-        <v>62861</v>
+        <v>64307</v>
       </c>
       <c r="D8" s="16">
-        <v>79789</v>
+        <v>81734</v>
       </c>
       <c r="E8" s="16">
-        <v>4020</v>
+        <v>4193</v>
       </c>
       <c r="F8" s="18">
-        <v>15991</v>
+        <v>15986</v>
       </c>
       <c r="G8" s="19">
-        <v>32464</v>
+        <v>33713</v>
       </c>
       <c r="H8" s="16">
-        <v>34064</v>
+        <v>34268</v>
       </c>
       <c r="I8" s="16">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="J8" s="18">
-        <v>12940</v>
+        <v>12983</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2576,28 +2578,28 @@
         <v>15</v>
       </c>
       <c r="C9" s="13">
-        <v>217885</v>
+        <v>222351</v>
       </c>
       <c r="D9" s="11">
-        <v>207488</v>
+        <v>212933</v>
       </c>
       <c r="E9" s="11">
-        <v>34031</v>
+        <v>37042</v>
       </c>
       <c r="F9" s="14">
-        <v>52416</v>
+        <v>52735</v>
       </c>
       <c r="G9" s="13">
-        <v>112597</v>
+        <v>116184</v>
       </c>
       <c r="H9" s="11">
-        <v>76945</v>
+        <v>78452</v>
       </c>
       <c r="I9" s="11">
-        <v>9656</v>
+        <v>9919</v>
       </c>
       <c r="J9" s="14">
-        <v>37480</v>
+        <v>37915</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -2608,28 +2610,28 @@
         <v>6</v>
       </c>
       <c r="C10" s="19">
-        <v>41295</v>
+        <v>42501</v>
       </c>
       <c r="D10" s="16">
-        <v>49366</v>
+        <v>50878</v>
       </c>
       <c r="E10" s="16">
-        <v>3170</v>
+        <v>3534</v>
       </c>
       <c r="F10" s="18">
-        <v>26610</v>
+        <v>27093</v>
       </c>
       <c r="G10" s="19">
-        <v>14838</v>
+        <v>15374</v>
       </c>
       <c r="H10" s="16">
-        <v>26592</v>
+        <v>26808</v>
       </c>
       <c r="I10" s="16">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="J10" s="18">
-        <v>16849</v>
+        <v>16974</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -2640,28 +2642,28 @@
         <v>7</v>
       </c>
       <c r="C11" s="13">
-        <v>269508</v>
+        <v>274276</v>
       </c>
       <c r="D11" s="11">
-        <v>241162</v>
+        <v>263152</v>
       </c>
       <c r="E11" s="11">
-        <v>53465</v>
+        <v>55142</v>
       </c>
       <c r="F11" s="14">
-        <v>98426</v>
+        <v>99861</v>
       </c>
       <c r="G11" s="13">
-        <v>101306</v>
+        <v>109575</v>
       </c>
       <c r="H11" s="11">
-        <v>103288</v>
+        <v>103849</v>
       </c>
       <c r="I11" s="11">
-        <v>30932</v>
+        <v>31056</v>
       </c>
       <c r="J11" s="14">
-        <v>82476</v>
+        <v>82979</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -2672,28 +2674,28 @@
         <v>8</v>
       </c>
       <c r="C12" s="19">
-        <v>482273</v>
+        <v>499111</v>
       </c>
       <c r="D12" s="16">
-        <v>723149</v>
+        <v>745856</v>
       </c>
       <c r="E12" s="16">
-        <v>26100</v>
+        <v>26873</v>
       </c>
       <c r="F12" s="18">
-        <v>191827</v>
+        <v>193249</v>
       </c>
       <c r="G12" s="19">
-        <v>182859</v>
+        <v>192638</v>
       </c>
       <c r="H12" s="16">
-        <v>312708</v>
+        <v>313920</v>
       </c>
       <c r="I12" s="16">
-        <v>15155</v>
+        <v>15283</v>
       </c>
       <c r="J12" s="18">
-        <v>151297</v>
+        <v>151990</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -2704,28 +2706,28 @@
         <v>12</v>
       </c>
       <c r="C13" s="13">
-        <v>113297</v>
+        <v>119165</v>
       </c>
       <c r="D13" s="11">
-        <v>177842</v>
+        <v>184660</v>
       </c>
       <c r="E13" s="11">
-        <v>7810</v>
+        <v>9068</v>
       </c>
       <c r="F13" s="14">
-        <v>36595</v>
+        <v>36789</v>
       </c>
       <c r="G13" s="13">
-        <v>52877</v>
+        <v>52918</v>
       </c>
       <c r="H13" s="11">
-        <v>58707</v>
+        <v>59299</v>
       </c>
       <c r="I13" s="11">
         <v>97</v>
       </c>
       <c r="J13" s="14">
-        <v>32290</v>
+        <v>32291</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -2736,28 +2738,28 @@
         <v>13</v>
       </c>
       <c r="C14" s="19">
-        <v>46692</v>
+        <v>48166</v>
       </c>
       <c r="D14" s="16">
-        <v>31493</v>
+        <v>32437</v>
       </c>
       <c r="E14" s="16">
-        <v>3106</v>
+        <v>3469</v>
       </c>
       <c r="F14" s="18">
-        <v>11420</v>
+        <v>11737</v>
       </c>
       <c r="G14" s="19">
-        <v>21429</v>
+        <v>21938</v>
       </c>
       <c r="H14" s="16">
-        <v>7932</v>
+        <v>8123</v>
       </c>
       <c r="I14" s="16">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J14" s="18">
-        <v>9608</v>
+        <v>9609</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -2768,28 +2770,28 @@
         <v>9</v>
       </c>
       <c r="C15" s="13">
-        <v>124235</v>
+        <v>125269</v>
       </c>
       <c r="D15" s="11">
-        <v>120387</v>
+        <v>122045</v>
       </c>
       <c r="E15" s="11">
-        <v>19500</v>
+        <v>20874</v>
       </c>
       <c r="F15" s="14">
         <v>33995</v>
       </c>
       <c r="G15" s="13">
-        <v>59695</v>
+        <v>63508</v>
       </c>
       <c r="H15" s="11">
-        <v>55222</v>
+        <v>56328</v>
       </c>
       <c r="I15" s="11">
-        <v>8696</v>
+        <v>8884</v>
       </c>
       <c r="J15" s="14">
-        <v>21563</v>
+        <v>21953</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -2800,28 +2802,28 @@
         <v>10</v>
       </c>
       <c r="C16" s="19">
-        <v>60501</v>
+        <v>64351</v>
       </c>
       <c r="D16" s="16">
-        <v>74941</v>
+        <v>76096</v>
       </c>
       <c r="E16" s="16">
-        <v>8165</v>
+        <v>8695</v>
       </c>
       <c r="F16" s="18">
-        <v>32580</v>
+        <v>32953</v>
       </c>
       <c r="G16" s="19">
-        <v>26776</v>
+        <v>28093</v>
       </c>
       <c r="H16" s="16">
-        <v>32258</v>
+        <v>32514</v>
       </c>
       <c r="I16" s="16">
-        <v>3561</v>
+        <v>3610</v>
       </c>
       <c r="J16" s="18">
-        <v>20945</v>
+        <v>21310</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -2832,28 +2834,28 @@
         <v>11</v>
       </c>
       <c r="C17" s="13">
-        <v>104969</v>
+        <v>110702</v>
       </c>
       <c r="D17" s="11">
-        <v>100811</v>
+        <v>103009</v>
       </c>
       <c r="E17" s="11">
-        <v>12136</v>
+        <v>12748</v>
       </c>
       <c r="F17" s="14">
-        <v>56175</v>
+        <v>56297</v>
       </c>
       <c r="G17" s="13">
-        <v>41736</v>
+        <v>41876</v>
       </c>
       <c r="H17" s="11">
-        <v>37155</v>
+        <v>37375</v>
       </c>
       <c r="I17" s="11">
-        <v>8897</v>
+        <v>8911</v>
       </c>
       <c r="J17" s="14">
-        <v>42502</v>
+        <v>42632</v>
       </c>
       <c r="K17" s="32"/>
     </row>
@@ -2865,58 +2867,58 @@
         <v>14</v>
       </c>
       <c r="C18" s="16">
-        <v>84422</v>
+        <v>87759</v>
       </c>
       <c r="D18" s="16">
-        <v>73507</v>
+        <v>73941</v>
       </c>
       <c r="E18" s="16">
-        <v>16519</v>
+        <v>16893</v>
       </c>
       <c r="F18" s="18">
-        <v>25963</v>
+        <v>26237</v>
       </c>
       <c r="G18" s="16">
-        <v>45144</v>
+        <v>47193</v>
       </c>
       <c r="H18" s="16">
-        <v>33442</v>
+        <v>34115</v>
       </c>
       <c r="I18" s="16">
-        <v>3825</v>
+        <v>3882</v>
       </c>
       <c r="J18" s="18">
-        <v>16644</v>
+        <v>17271</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="D19" s="11">
+        <v>6064</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="H19" s="11">
+        <v>20</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2925,28 +2927,28 @@
         <v>19</v>
       </c>
       <c r="C20" s="49">
-        <v>2802360</v>
+        <v>2889852</v>
       </c>
       <c r="D20" s="50">
-        <v>2973793</v>
+        <v>3065737</v>
       </c>
       <c r="E20" s="50">
-        <v>324003</v>
+        <v>343067</v>
       </c>
       <c r="F20" s="51">
-        <v>880699</v>
+        <v>888407</v>
       </c>
       <c r="G20" s="49">
-        <v>1291125</v>
+        <v>1337635</v>
       </c>
       <c r="H20" s="50">
-        <v>1221239</v>
+        <v>1231953</v>
       </c>
       <c r="I20" s="50">
-        <v>105188</v>
+        <v>106375</v>
       </c>
       <c r="J20" s="51">
-        <v>682504</v>
+        <v>687656</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -2966,7 +2968,7 @@
     </row>
     <row r="25" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="56" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B25" s="56"/>
       <c r="C25" s="56"/>
@@ -2999,10 +3001,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926B42D2-7956-44E7-BD5B-5AF896796AC0}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3060,13 +3062,13 @@
         <v>44194</v>
       </c>
       <c r="B4" s="33">
-        <v>42652</v>
+        <v>42651</v>
       </c>
       <c r="C4" s="33">
         <v>0</v>
       </c>
       <c r="D4" s="33">
-        <v>42652</v>
+        <v>42651</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3074,13 +3076,13 @@
         <v>44195</v>
       </c>
       <c r="B5" s="33">
-        <v>58002</v>
+        <v>58001</v>
       </c>
       <c r="C5" s="33">
         <v>0</v>
       </c>
       <c r="D5" s="33">
-        <v>58002</v>
+        <v>58001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3102,13 +3104,13 @@
         <v>44197</v>
       </c>
       <c r="B7" s="33">
-        <v>24750</v>
+        <v>24749</v>
       </c>
       <c r="C7" s="33">
         <v>0</v>
       </c>
       <c r="D7" s="33">
-        <v>24750</v>
+        <v>24749</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3144,13 +3146,13 @@
         <v>44200</v>
       </c>
       <c r="B10" s="33">
-        <v>48686</v>
+        <v>48685</v>
       </c>
       <c r="C10" s="33">
         <v>0</v>
       </c>
       <c r="D10" s="33">
-        <v>48686</v>
+        <v>48685</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -3158,13 +3160,13 @@
         <v>44201</v>
       </c>
       <c r="B11" s="33">
-        <v>52458</v>
+        <v>52456</v>
       </c>
       <c r="C11" s="33">
         <v>0</v>
       </c>
       <c r="D11" s="33">
-        <v>52458</v>
+        <v>52456</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -3172,13 +3174,13 @@
         <v>44202</v>
       </c>
       <c r="B12" s="33">
-        <v>59170</v>
+        <v>59167</v>
       </c>
       <c r="C12" s="33">
         <v>0</v>
       </c>
       <c r="D12" s="33">
-        <v>59170</v>
+        <v>59167</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -3186,13 +3188,13 @@
         <v>44203</v>
       </c>
       <c r="B13" s="33">
-        <v>58465</v>
+        <v>58462</v>
       </c>
       <c r="C13" s="33">
         <v>0</v>
       </c>
       <c r="D13" s="33">
-        <v>58465</v>
+        <v>58462</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3200,13 +3202,13 @@
         <v>44204</v>
       </c>
       <c r="B14" s="33">
-        <v>60447</v>
+        <v>60445</v>
       </c>
       <c r="C14" s="33">
         <v>0</v>
       </c>
       <c r="D14" s="33">
-        <v>60447</v>
+        <v>60445</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -3214,13 +3216,13 @@
         <v>44205</v>
       </c>
       <c r="B15" s="33">
-        <v>57326</v>
+        <v>57323</v>
       </c>
       <c r="C15" s="33">
         <v>0</v>
       </c>
       <c r="D15" s="33">
-        <v>57326</v>
+        <v>57323</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -3228,13 +3230,13 @@
         <v>44206</v>
       </c>
       <c r="B16" s="33">
-        <v>33281</v>
+        <v>33280</v>
       </c>
       <c r="C16" s="33">
         <v>0</v>
       </c>
       <c r="D16" s="33">
-        <v>33281</v>
+        <v>33280</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -3242,13 +3244,13 @@
         <v>44207</v>
       </c>
       <c r="B17" s="33">
-        <v>65668</v>
+        <v>65667</v>
       </c>
       <c r="C17" s="33">
         <v>0</v>
       </c>
       <c r="D17" s="33">
-        <v>65668</v>
+        <v>65667</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -3256,13 +3258,13 @@
         <v>44208</v>
       </c>
       <c r="B18" s="33">
-        <v>82088</v>
+        <v>82084</v>
       </c>
       <c r="C18" s="33">
         <v>0</v>
       </c>
       <c r="D18" s="33">
-        <v>82088</v>
+        <v>82084</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -3270,13 +3272,13 @@
         <v>44209</v>
       </c>
       <c r="B19" s="33">
-        <v>99087</v>
+        <v>99086</v>
       </c>
       <c r="C19" s="33">
         <v>0</v>
       </c>
       <c r="D19" s="33">
-        <v>99087</v>
+        <v>99086</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -3284,13 +3286,13 @@
         <v>44210</v>
       </c>
       <c r="B20" s="33">
-        <v>100114</v>
+        <v>100115</v>
       </c>
       <c r="C20" s="33">
         <v>114</v>
       </c>
       <c r="D20" s="33">
-        <v>100228</v>
+        <v>100229</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -3298,13 +3300,13 @@
         <v>44211</v>
       </c>
       <c r="B21" s="33">
-        <v>92397</v>
+        <v>92396</v>
       </c>
       <c r="C21" s="33">
         <v>428</v>
       </c>
       <c r="D21" s="33">
-        <v>92825</v>
+        <v>92824</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -3312,13 +3314,13 @@
         <v>44212</v>
       </c>
       <c r="B22" s="33">
-        <v>56708</v>
+        <v>56703</v>
       </c>
       <c r="C22" s="33">
         <v>397</v>
       </c>
       <c r="D22" s="33">
-        <v>57105</v>
+        <v>57100</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3326,13 +3328,13 @@
         <v>44213</v>
       </c>
       <c r="B23" s="33">
-        <v>30899</v>
+        <v>30897</v>
       </c>
       <c r="C23" s="33">
-        <v>13612</v>
+        <v>13611</v>
       </c>
       <c r="D23" s="33">
-        <v>44511</v>
+        <v>44508</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -3340,13 +3342,13 @@
         <v>44214</v>
       </c>
       <c r="B24" s="33">
-        <v>57986</v>
+        <v>57985</v>
       </c>
       <c r="C24" s="33">
         <v>16372</v>
       </c>
       <c r="D24" s="33">
-        <v>74358</v>
+        <v>74357</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -3354,13 +3356,13 @@
         <v>44215</v>
       </c>
       <c r="B25" s="33">
-        <v>68174</v>
+        <v>68172</v>
       </c>
       <c r="C25" s="33">
         <v>27229</v>
       </c>
       <c r="D25" s="33">
-        <v>95403</v>
+        <v>95401</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -3368,13 +3370,13 @@
         <v>44216</v>
       </c>
       <c r="B26" s="33">
-        <v>78286</v>
+        <v>78284</v>
       </c>
       <c r="C26" s="33">
         <v>50656</v>
       </c>
       <c r="D26" s="33">
-        <v>128942</v>
+        <v>128940</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -3382,13 +3384,13 @@
         <v>44217</v>
       </c>
       <c r="B27" s="33">
-        <v>60698</v>
+        <v>60697</v>
       </c>
       <c r="C27" s="33">
         <v>35435</v>
       </c>
       <c r="D27" s="33">
-        <v>96133</v>
+        <v>96132</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -3396,13 +3398,13 @@
         <v>44218</v>
       </c>
       <c r="B28" s="33">
-        <v>84246</v>
+        <v>84252</v>
       </c>
       <c r="C28" s="33">
-        <v>31288</v>
+        <v>31358</v>
       </c>
       <c r="D28" s="33">
-        <v>115534</v>
+        <v>115610</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -3424,13 +3426,13 @@
         <v>44220</v>
       </c>
       <c r="B30" s="33">
-        <v>38212</v>
+        <v>38211</v>
       </c>
       <c r="C30" s="33">
         <v>28089</v>
       </c>
       <c r="D30" s="33">
-        <v>66301</v>
+        <v>66300</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -3438,13 +3440,13 @@
         <v>44221</v>
       </c>
       <c r="B31" s="33">
-        <v>58193</v>
+        <v>58192</v>
       </c>
       <c r="C31" s="33">
         <v>39738</v>
       </c>
       <c r="D31" s="33">
-        <v>97931</v>
+        <v>97930</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -3452,13 +3454,13 @@
         <v>44222</v>
       </c>
       <c r="B32" s="33">
-        <v>53110</v>
+        <v>53109</v>
       </c>
       <c r="C32" s="33">
-        <v>49611</v>
+        <v>49610</v>
       </c>
       <c r="D32" s="33">
-        <v>102721</v>
+        <v>102719</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -3466,13 +3468,13 @@
         <v>44223</v>
       </c>
       <c r="B33" s="33">
-        <v>54052</v>
+        <v>54054</v>
       </c>
       <c r="C33" s="33">
-        <v>59286</v>
+        <v>59285</v>
       </c>
       <c r="D33" s="33">
-        <v>113338</v>
+        <v>113339</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3497,10 +3499,10 @@
         <v>55982</v>
       </c>
       <c r="C35" s="33">
-        <v>53759</v>
+        <v>53757</v>
       </c>
       <c r="D35" s="33">
-        <v>109741</v>
+        <v>109739</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -3522,13 +3524,13 @@
         <v>44227</v>
       </c>
       <c r="B37" s="33">
-        <v>31326</v>
+        <v>31325</v>
       </c>
       <c r="C37" s="33">
         <v>31380</v>
       </c>
       <c r="D37" s="33">
-        <v>62706</v>
+        <v>62705</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -3536,13 +3538,13 @@
         <v>44228</v>
       </c>
       <c r="B38" s="33">
-        <v>50094</v>
+        <v>50092</v>
       </c>
       <c r="C38" s="33">
-        <v>65862</v>
+        <v>65861</v>
       </c>
       <c r="D38" s="33">
-        <v>115956</v>
+        <v>115953</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -3550,13 +3552,13 @@
         <v>44229</v>
       </c>
       <c r="B39" s="33">
-        <v>57930</v>
+        <v>57927</v>
       </c>
       <c r="C39" s="33">
-        <v>69749</v>
+        <v>69748</v>
       </c>
       <c r="D39" s="33">
-        <v>127679</v>
+        <v>127675</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -3564,13 +3566,13 @@
         <v>44230</v>
       </c>
       <c r="B40" s="33">
-        <v>57963</v>
+        <v>57977</v>
       </c>
       <c r="C40" s="33">
-        <v>84655</v>
+        <v>84742</v>
       </c>
       <c r="D40" s="33">
-        <v>142618</v>
+        <v>142719</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -3578,13 +3580,13 @@
         <v>44231</v>
       </c>
       <c r="B41" s="33">
-        <v>63142</v>
+        <v>63139</v>
       </c>
       <c r="C41" s="33">
-        <v>72640</v>
+        <v>72687</v>
       </c>
       <c r="D41" s="33">
-        <v>135782</v>
+        <v>135826</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -3592,13 +3594,13 @@
         <v>44232</v>
       </c>
       <c r="B42" s="33">
-        <v>59739</v>
+        <v>59865</v>
       </c>
       <c r="C42" s="33">
         <v>73707</v>
       </c>
       <c r="D42" s="33">
-        <v>133446</v>
+        <v>133572</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -3606,13 +3608,13 @@
         <v>44233</v>
       </c>
       <c r="B43" s="33">
-        <v>48595</v>
+        <v>48615</v>
       </c>
       <c r="C43" s="33">
-        <v>55159</v>
+        <v>55255</v>
       </c>
       <c r="D43" s="33">
-        <v>103754</v>
+        <v>103870</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -3634,13 +3636,13 @@
         <v>44235</v>
       </c>
       <c r="B45" s="33">
-        <v>54802</v>
+        <v>54801</v>
       </c>
       <c r="C45" s="33">
         <v>51617</v>
       </c>
       <c r="D45" s="33">
-        <v>106419</v>
+        <v>106418</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -3648,13 +3650,13 @@
         <v>44236</v>
       </c>
       <c r="B46" s="33">
-        <v>59648</v>
+        <v>59665</v>
       </c>
       <c r="C46" s="33">
-        <v>65081</v>
+        <v>65161</v>
       </c>
       <c r="D46" s="33">
-        <v>124729</v>
+        <v>124826</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -3662,13 +3664,13 @@
         <v>44237</v>
       </c>
       <c r="B47" s="33">
-        <v>75273</v>
+        <v>75272</v>
       </c>
       <c r="C47" s="33">
-        <v>74922</v>
+        <v>75113</v>
       </c>
       <c r="D47" s="33">
-        <v>150195</v>
+        <v>150385</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -3676,13 +3678,13 @@
         <v>44238</v>
       </c>
       <c r="B48" s="33">
-        <v>71451</v>
+        <v>71446</v>
       </c>
       <c r="C48" s="33">
         <v>72440</v>
       </c>
       <c r="D48" s="33">
-        <v>143891</v>
+        <v>143886</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -3690,13 +3692,13 @@
         <v>44239</v>
       </c>
       <c r="B49" s="33">
-        <v>80088</v>
+        <v>80124</v>
       </c>
       <c r="C49" s="33">
-        <v>78357</v>
+        <v>78379</v>
       </c>
       <c r="D49" s="33">
-        <v>158445</v>
+        <v>158503</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -3704,13 +3706,13 @@
         <v>44240</v>
       </c>
       <c r="B50" s="33">
-        <v>63263</v>
+        <v>63273</v>
       </c>
       <c r="C50" s="33">
         <v>46644</v>
       </c>
       <c r="D50" s="33">
-        <v>109907</v>
+        <v>109917</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -3718,13 +3720,13 @@
         <v>44241</v>
       </c>
       <c r="B51" s="33">
-        <v>39774</v>
+        <v>39787</v>
       </c>
       <c r="C51" s="33">
-        <v>26982</v>
+        <v>26981</v>
       </c>
       <c r="D51" s="33">
-        <v>66756</v>
+        <v>66768</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -3732,13 +3734,13 @@
         <v>44242</v>
       </c>
       <c r="B52" s="33">
-        <v>70779</v>
+        <v>70784</v>
       </c>
       <c r="C52" s="33">
-        <v>56021</v>
+        <v>56019</v>
       </c>
       <c r="D52" s="33">
-        <v>126800</v>
+        <v>126803</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3746,13 +3748,13 @@
         <v>44243</v>
       </c>
       <c r="B53" s="33">
-        <v>81516</v>
+        <v>81520</v>
       </c>
       <c r="C53" s="33">
-        <v>54755</v>
+        <v>54757</v>
       </c>
       <c r="D53" s="33">
-        <v>136271</v>
+        <v>136277</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3760,13 +3762,13 @@
         <v>44244</v>
       </c>
       <c r="B54" s="33">
-        <v>94511</v>
+        <v>94653</v>
       </c>
       <c r="C54" s="33">
         <v>54646</v>
       </c>
       <c r="D54" s="33">
-        <v>149157</v>
+        <v>149299</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -3774,13 +3776,13 @@
         <v>44245</v>
       </c>
       <c r="B55" s="33">
-        <v>93347</v>
+        <v>93570</v>
       </c>
       <c r="C55" s="33">
-        <v>52045</v>
+        <v>52046</v>
       </c>
       <c r="D55" s="33">
-        <v>145392</v>
+        <v>145616</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3788,13 +3790,13 @@
         <v>44246</v>
       </c>
       <c r="B56" s="33">
-        <v>96861</v>
+        <v>97188</v>
       </c>
       <c r="C56" s="33">
-        <v>53497</v>
+        <v>53496</v>
       </c>
       <c r="D56" s="33">
-        <v>150358</v>
+        <v>150684</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3802,13 +3804,13 @@
         <v>44247</v>
       </c>
       <c r="B57" s="33">
-        <v>74925</v>
+        <v>74961</v>
       </c>
       <c r="C57" s="33">
         <v>37662</v>
       </c>
       <c r="D57" s="33">
-        <v>112587</v>
+        <v>112623</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3816,13 +3818,13 @@
         <v>44248</v>
       </c>
       <c r="B58" s="33">
-        <v>56636</v>
+        <v>56633</v>
       </c>
       <c r="C58" s="33">
-        <v>28939</v>
+        <v>28938</v>
       </c>
       <c r="D58" s="33">
-        <v>85575</v>
+        <v>85571</v>
       </c>
     </row>
     <row r="59" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3830,13 +3832,13 @@
         <v>44249</v>
       </c>
       <c r="B59" s="33">
-        <v>99008</v>
+        <v>99204</v>
       </c>
       <c r="C59" s="33">
-        <v>52976</v>
+        <v>52972</v>
       </c>
       <c r="D59" s="33">
-        <v>151984</v>
+        <v>152176</v>
       </c>
     </row>
     <row r="60" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3844,13 +3846,13 @@
         <v>44250</v>
       </c>
       <c r="B60" s="33">
-        <v>104008</v>
+        <v>104259</v>
       </c>
       <c r="C60" s="33">
-        <v>55640</v>
+        <v>55643</v>
       </c>
       <c r="D60" s="33">
-        <v>159648</v>
+        <v>159902</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3858,13 +3860,13 @@
         <v>44251</v>
       </c>
       <c r="B61" s="33">
-        <v>116539</v>
+        <v>116796</v>
       </c>
       <c r="C61" s="33">
-        <v>57936</v>
+        <v>57949</v>
       </c>
       <c r="D61" s="33">
-        <v>174475</v>
+        <v>174745</v>
       </c>
     </row>
     <row r="62" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3872,13 +3874,13 @@
         <v>44252</v>
       </c>
       <c r="B62" s="33">
-        <v>127064</v>
+        <v>127154</v>
       </c>
       <c r="C62" s="33">
-        <v>52364</v>
+        <v>52369</v>
       </c>
       <c r="D62" s="33">
-        <v>179428</v>
+        <v>179523</v>
       </c>
     </row>
     <row r="63" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3886,13 +3888,13 @@
         <v>44253</v>
       </c>
       <c r="B63" s="33">
-        <v>135976</v>
+        <v>136522</v>
       </c>
       <c r="C63" s="33">
-        <v>58667</v>
+        <v>58838</v>
       </c>
       <c r="D63" s="33">
-        <v>194643</v>
+        <v>195360</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3900,13 +3902,13 @@
         <v>44254</v>
       </c>
       <c r="B64" s="33">
-        <v>107584</v>
+        <v>107836</v>
       </c>
       <c r="C64" s="33">
-        <v>38763</v>
+        <v>38858</v>
       </c>
       <c r="D64" s="33">
-        <v>146347</v>
+        <v>146694</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3914,13 +3916,13 @@
         <v>44255</v>
       </c>
       <c r="B65" s="33">
-        <v>85652</v>
+        <v>85649</v>
       </c>
       <c r="C65" s="33">
         <v>27932</v>
       </c>
       <c r="D65" s="33">
-        <v>113584</v>
+        <v>113581</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -3928,13 +3930,13 @@
         <v>44256</v>
       </c>
       <c r="B66" s="33">
-        <v>140571</v>
+        <v>141232</v>
       </c>
       <c r="C66" s="33">
         <v>50255</v>
       </c>
       <c r="D66" s="33">
-        <v>190826</v>
+        <v>191487</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -3942,13 +3944,13 @@
         <v>44257</v>
       </c>
       <c r="B67" s="33">
-        <v>158615</v>
+        <v>159571</v>
       </c>
       <c r="C67" s="33">
         <v>55657</v>
       </c>
       <c r="D67" s="33">
-        <v>214272</v>
+        <v>215228</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -3956,13 +3958,13 @@
         <v>44258</v>
       </c>
       <c r="B68" s="33">
-        <v>172178</v>
+        <v>172865</v>
       </c>
       <c r="C68" s="33">
-        <v>67189</v>
+        <v>67227</v>
       </c>
       <c r="D68" s="33">
-        <v>239367</v>
+        <v>240092</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -3970,13 +3972,13 @@
         <v>44259</v>
       </c>
       <c r="B69" s="33">
-        <v>175135</v>
+        <v>175784</v>
       </c>
       <c r="C69" s="33">
         <v>61767</v>
       </c>
       <c r="D69" s="33">
-        <v>236902</v>
+        <v>237551</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -3984,13 +3986,13 @@
         <v>44260</v>
       </c>
       <c r="B70" s="33">
-        <v>184164</v>
+        <v>185975</v>
       </c>
       <c r="C70" s="33">
-        <v>63186</v>
+        <v>63263</v>
       </c>
       <c r="D70" s="33">
-        <v>247350</v>
+        <v>249238</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -3998,13 +4000,13 @@
         <v>44261</v>
       </c>
       <c r="B71" s="33">
-        <v>144936</v>
+        <v>145934</v>
       </c>
       <c r="C71" s="33">
-        <v>47131</v>
+        <v>47244</v>
       </c>
       <c r="D71" s="33">
-        <v>192067</v>
+        <v>193178</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -4012,134 +4014,172 @@
         <v>44262</v>
       </c>
       <c r="B72" s="33">
-        <v>112991</v>
+        <v>113180</v>
       </c>
       <c r="C72" s="33">
-        <v>34265.5</v>
+        <v>34371.5</v>
       </c>
       <c r="D72" s="33">
-        <v>147256.5</v>
+        <v>147551.5</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="38">
         <v>44263</v>
       </c>
-      <c r="B73" s="54">
-        <v>176692</v>
-      </c>
-      <c r="C73" s="54">
-        <v>53095.5</v>
-      </c>
-      <c r="D73" s="54">
-        <v>229787.5</v>
+      <c r="B73" s="52">
+        <v>177365</v>
+      </c>
+      <c r="C73" s="52">
+        <v>53158.5</v>
+      </c>
+      <c r="D73" s="52">
+        <v>230523.5</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="38">
         <v>44264</v>
       </c>
-      <c r="B74" s="54">
-        <v>189562</v>
-      </c>
-      <c r="C74" s="54">
-        <v>54962</v>
-      </c>
-      <c r="D74" s="54">
-        <v>244524</v>
+      <c r="B74" s="52">
+        <v>190903</v>
+      </c>
+      <c r="C74" s="52">
+        <v>55045</v>
+      </c>
+      <c r="D74" s="52">
+        <v>245948</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="38">
         <v>44265</v>
       </c>
-      <c r="B75" s="54">
-        <v>204928</v>
-      </c>
-      <c r="C75" s="54">
-        <v>66591</v>
-      </c>
-      <c r="D75" s="54">
-        <v>271519</v>
+      <c r="B75" s="52">
+        <v>206910</v>
+      </c>
+      <c r="C75" s="52">
+        <v>66863</v>
+      </c>
+      <c r="D75" s="52">
+        <v>273773</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="38">
         <v>44266</v>
       </c>
-      <c r="B76" s="54">
-        <v>217686</v>
-      </c>
-      <c r="C76" s="54">
-        <v>62169</v>
-      </c>
-      <c r="D76" s="54">
-        <v>279855</v>
+      <c r="B76" s="52">
+        <v>220897</v>
+      </c>
+      <c r="C76" s="52">
+        <v>62666</v>
+      </c>
+      <c r="D76" s="52">
+        <v>283563</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="38">
         <v>44267</v>
       </c>
-      <c r="B77" s="54">
-        <v>203891</v>
-      </c>
-      <c r="C77" s="54">
-        <v>67671</v>
-      </c>
-      <c r="D77" s="54">
-        <v>271562</v>
+      <c r="B77" s="52">
+        <v>218516</v>
+      </c>
+      <c r="C77" s="52">
+        <v>68455</v>
+      </c>
+      <c r="D77" s="52">
+        <v>286971</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="38">
         <v>44268</v>
       </c>
-      <c r="B78" s="54">
-        <v>177920</v>
-      </c>
-      <c r="C78" s="54">
-        <v>47794</v>
-      </c>
-      <c r="D78" s="54">
-        <v>225714</v>
+      <c r="B78" s="52">
+        <v>182850</v>
+      </c>
+      <c r="C78" s="52">
+        <v>47848</v>
+      </c>
+      <c r="D78" s="52">
+        <v>230698</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="38">
         <v>44269</v>
       </c>
-      <c r="B79" s="54">
-        <v>128148</v>
-      </c>
-      <c r="C79" s="54">
-        <v>35097</v>
-      </c>
-      <c r="D79" s="54">
-        <v>163245</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="55"/>
-      <c r="B80" s="55"/>
-      <c r="C80" s="53"/>
-      <c r="D80" s="53"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="43" t="s">
+      <c r="B79" s="52">
+        <v>128880</v>
+      </c>
+      <c r="C79" s="52">
+        <v>35111</v>
+      </c>
+      <c r="D79" s="52">
+        <v>163991</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="38">
+        <v>44270</v>
+      </c>
+      <c r="B80" s="52">
+        <v>169080</v>
+      </c>
+      <c r="C80" s="52">
+        <v>56773</v>
+      </c>
+      <c r="D80" s="52">
+        <v>225853</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="53"/>
+      <c r="B81" s="53"/>
+      <c r="C81" s="53"/>
+      <c r="D81" s="53"/>
+    </row>
+    <row r="82" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="53"/>
+      <c r="B82" s="53"/>
+      <c r="C82" s="53"/>
+      <c r="D82" s="53"/>
+    </row>
+    <row r="83" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="53"/>
+      <c r="B83" s="53"/>
+      <c r="C83" s="53"/>
+      <c r="D83" s="53"/>
+    </row>
+    <row r="84" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="53"/>
+      <c r="B84" s="53"/>
+      <c r="C84" s="53"/>
+      <c r="D84" s="53"/>
+    </row>
+    <row r="85" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="53"/>
+      <c r="B85" s="53"/>
+      <c r="C85" s="53"/>
+      <c r="D85" s="53"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B81" s="33">
+      <c r="B86" s="33">
         <f>SUM(B2:B80)</f>
-        <v>6507159</v>
-      </c>
-      <c r="C81" s="33">
+        <v>6712195</v>
+      </c>
+      <c r="C86" s="33">
         <f>SUM(C2:C80)</f>
-        <v>2891951</v>
-      </c>
-      <c r="D81" s="33">
+        <v>2951692</v>
+      </c>
+      <c r="D86" s="33">
         <f>SUM(D2:D80)</f>
-        <v>9399110</v>
+        <v>9663887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>